<commit_message>
clean up code, run on more subjects
</commit_message>
<xml_diff>
--- a/HR_Data/LWP2_0011_FirstBeat_RR_raw_data_by_task.xlsx
+++ b/HR_Data/LWP2_0011_FirstBeat_RR_raw_data_by_task.xlsx
@@ -13,24 +13,24 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Task1 Relaxing Music1" sheetId="2" r:id="rId2"/>
-    <sheet name="Task2 Relaxing Pic1" sheetId="3" r:id="rId3"/>
-    <sheet name="Task3 EMA1" sheetId="4" r:id="rId4"/>
-    <sheet name="Task4 IAPS" sheetId="5" r:id="rId5"/>
-    <sheet name="Task5 StressPic1" sheetId="6" r:id="rId6"/>
-    <sheet name="Task6 EMA2" sheetId="7" r:id="rId7"/>
-    <sheet name="Task7 Relaxing Music2" sheetId="8" r:id="rId8"/>
-    <sheet name="Task8 Relaxing Pic2" sheetId="9" r:id="rId9"/>
-    <sheet name="Task9 EMA3" sheetId="10" r:id="rId10"/>
-    <sheet name="Task10 Biking" sheetId="11" r:id="rId11"/>
-    <sheet name="Task11 Relaxing Music3" sheetId="12" r:id="rId12"/>
-    <sheet name="Task12 NeutralPic" sheetId="13" r:id="rId13"/>
-    <sheet name="Task13 EMA4" sheetId="14" r:id="rId14"/>
-    <sheet name="Task14 MentalMath" sheetId="15" r:id="rId15"/>
-    <sheet name="Task15 Stroop" sheetId="16" r:id="rId16"/>
-    <sheet name="Task16 StressPic2" sheetId="17" r:id="rId17"/>
-    <sheet name="Task17 EMA5" sheetId="18" r:id="rId18"/>
-    <sheet name="Task18 March" sheetId="19" r:id="rId19"/>
+    <sheet name="Task1_RelaxingMusic1" sheetId="2" r:id="rId2"/>
+    <sheet name="Task2_RelaxingPic1" sheetId="3" r:id="rId3"/>
+    <sheet name="Task3_EMA1" sheetId="4" r:id="rId4"/>
+    <sheet name="Task4_IAPS" sheetId="5" r:id="rId5"/>
+    <sheet name="Task5_StressPic1" sheetId="6" r:id="rId6"/>
+    <sheet name="Task6_EMA2" sheetId="7" r:id="rId7"/>
+    <sheet name="Task7_RelaxingMusic2" sheetId="8" r:id="rId8"/>
+    <sheet name="Task8_RelaxingPic2" sheetId="9" r:id="rId9"/>
+    <sheet name="Task9_EMA3" sheetId="10" r:id="rId10"/>
+    <sheet name="Task10_Biking" sheetId="11" r:id="rId11"/>
+    <sheet name="Task11_RelaxingMusic3" sheetId="12" r:id="rId12"/>
+    <sheet name="Task12_NeutralPic" sheetId="13" r:id="rId13"/>
+    <sheet name="Task13_EMA4" sheetId="14" r:id="rId14"/>
+    <sheet name="Task14_MentalMath" sheetId="15" r:id="rId15"/>
+    <sheet name="Task15_Stroop" sheetId="16" r:id="rId16"/>
+    <sheet name="Task16_StressPic2" sheetId="17" r:id="rId17"/>
+    <sheet name="Task17_EMA5" sheetId="18" r:id="rId18"/>
+    <sheet name="Task18_March" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>

</xml_diff>